<commit_message>
update excel template and rendering
</commit_message>
<xml_diff>
--- a/cgadmin/invoice/templates/invoice.xlsx
+++ b/cgadmin/invoice/templates/invoice.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="27729"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-33600" yWindow="7800" windowWidth="33600" windowHeight="20540"/>
+    <workbookView xWindow="3960" yWindow="4980" windowWidth="25600" windowHeight="16060"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="26">
   <si>
     <t>Fakturaunderlag</t>
   </si>
@@ -57,12 +57,6 @@
     <t>Fakturaadress</t>
   </si>
   <si>
-    <t>Avtaltets diarienummer</t>
-  </si>
-  <si>
-    <t>4-1378/2015</t>
-  </si>
-  <si>
     <t>Prov</t>
   </si>
   <si>
@@ -100,6 +94,9 @@
   </si>
   <si>
     <t>Ankomstdatum</t>
+  </si>
+  <si>
+    <t>Avser kostnader i projekt med</t>
   </si>
 </sst>
 </file>
@@ -110,7 +107,7 @@
     <numFmt numFmtId="164" formatCode="#\ \k\r"/>
     <numFmt numFmtId="165" formatCode="yyyy/mm/dd;@"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -163,6 +160,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -207,11 +212,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -225,6 +235,8 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -234,10 +246,14 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="7">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -534,7 +550,7 @@
   <dimension ref="A1:F53"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -543,41 +559,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9"/>
+      <c r="B1" s="11"/>
       <c r="C1" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="18">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="10"/>
+      <c r="B2" s="12"/>
       <c r="E2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
+      <c r="A5" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="13"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="4" t="s">
@@ -592,7 +608,7 @@
         <v>5</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -608,7 +624,7 @@
         <v>8</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -616,25 +632,25 @@
         <v>9</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="B12" s="11"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
+      <c r="A12" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -642,7 +658,7 @@
         <v>8</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -650,15 +666,15 @@
         <v>10</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -666,50 +682,54 @@
         <v>11</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="11" t="s">
+      <c r="A19" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="13"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="11"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>13</v>
-      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="4"/>
+      <c r="C21" s="2"/>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="D23" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C23" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D23" s="3" t="s">
+      <c r="E23" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F23" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E23" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>19</v>
-      </c>
     </row>
     <row r="24" spans="1:6">
-      <c r="A24" s="12"/>
-      <c r="B24" s="13"/>
+      <c r="A24" s="9"/>
+      <c r="B24" s="10"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>

</xml_diff>